<commit_message>
feat: Last transection missing issue resolve
</commit_message>
<xml_diff>
--- a/employees_loaded.xlsx
+++ b/employees_loaded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1 Data Analysis Part 2\1 Shared Folder\Ticket Distribution\Ticket_Streamlit_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEA2B0B-A47C-43DC-B09A-DA027F572596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447CC64C-D477-41D2-ABAB-5972310C78D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F699083D-B6A8-4A33-9A60-164D10EA3BF2}"/>
   </bookViews>
@@ -18466,7 +18466,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -18846,7 +18846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1370B36A-A6C7-4AE7-86D3-7904C0AD1198}">
   <dimension ref="A1:B3308"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>